<commit_message>
Addedd population state discretization test
</commit_message>
<xml_diff>
--- a/Water Decision Model Data Inputs.xlsx
+++ b/Water Decision Model Data Inputs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahfletcher/Documents/MATLAB/Repository_SDP/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="689" activeTab="1"/>
+    <workbookView xWindow="7260" yWindow="3060" windowWidth="18340" windowHeight="10340" tabRatio="689" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Parameters" sheetId="3" r:id="rId1"/>
@@ -15,8 +20,11 @@
     <sheet name="Infrastructure Alternatives" sheetId="9" r:id="rId6"/>
     <sheet name="Data source info" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1509,6 +1517,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2125,7 +2138,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
@@ -2135,7 +2148,7 @@
     <col min="6" max="6" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="68" t="s">
         <v>177</v>
       </c>
@@ -2144,14 +2157,14 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>107</v>
       </c>
@@ -2181,7 +2194,7 @@
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
@@ -2201,7 +2214,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
@@ -2217,7 +2230,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
@@ -2235,7 +2248,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" customHeight="1">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
         <v>108</v>
       </c>
@@ -2245,7 +2258,7 @@
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="1:6" ht="24">
+    <row r="9" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="34" t="s">
         <v>109</v>
       </c>
@@ -2257,7 +2270,7 @@
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
     </row>
-    <row r="10" spans="1:6" ht="24">
+    <row r="10" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
         <v>97</v>
       </c>
@@ -2277,7 +2290,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24">
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
         <v>98</v>
       </c>
@@ -2295,7 +2308,7 @@
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="22" customHeight="1">
+    <row r="12" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
@@ -2311,7 +2324,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="26" customHeight="1">
+    <row r="13" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>21</v>
       </c>
@@ -2329,8 +2342,8 @@
       </c>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="18" customHeight="1"/>
-    <row r="15" spans="1:6" s="35" customFormat="1" ht="18" customHeight="1">
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:6" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="26" t="s">
         <v>50</v>
       </c>
@@ -2340,7 +2353,7 @@
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
     </row>
-    <row r="16" spans="1:6" ht="18" customHeight="1">
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="11" t="s">
         <v>24</v>
       </c>
@@ -2356,7 +2369,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="18" customHeight="1">
+    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
         <v>26</v>
       </c>
@@ -2372,7 +2385,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18" customHeight="1">
+    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2380,7 +2393,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="18" customHeight="1">
+    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="67" t="s">
         <v>29</v>
       </c>
@@ -2390,7 +2403,7 @@
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
     </row>
-    <row r="20" spans="1:6" ht="18" customHeight="1">
+    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
         <v>16</v>
       </c>
@@ -2404,7 +2417,7 @@
       </c>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="18" customHeight="1">
+    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
         <v>18</v>
       </c>
@@ -2416,7 +2429,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="18" customHeight="1">
+    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
         <v>21</v>
       </c>
@@ -2430,7 +2443,7 @@
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="18" customHeight="1">
+    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="11" t="s">
         <v>35</v>
       </c>
@@ -2442,7 +2455,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="18" customHeight="1">
+    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
         <v>14</v>
       </c>
@@ -2454,7 +2467,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="18" customHeight="1">
+    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="22"/>
       <c r="B25" s="23"/>
       <c r="C25" s="22"/>
@@ -2462,7 +2475,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="18" customHeight="1">
+    <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
@@ -2470,7 +2483,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="18" customHeight="1">
+    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -2478,18 +2491,13 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="18" customHeight="1"/>
-    <row r="29" spans="1:6" ht="18" customHeight="1"/>
-    <row r="30" spans="1:6" ht="18" customHeight="1"/>
+    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2497,11 +2505,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" customWidth="1"/>
@@ -2509,7 +2517,7 @@
     <col min="8" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15">
+    <row r="1" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>53</v>
       </c>
@@ -2524,7 +2532,7 @@
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
     </row>
-    <row r="2" spans="1:26" ht="15">
+    <row r="2" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="63"/>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
@@ -2550,7 +2558,7 @@
       <c r="X2" s="35"/>
       <c r="Y2" s="35"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="62" t="s">
         <v>168</v>
       </c>
@@ -2577,7 +2585,7 @@
       <c r="X3" s="35"/>
       <c r="Y3" s="35"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="62"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
@@ -2602,7 +2610,7 @@
       <c r="X4" s="35"/>
       <c r="Y4" s="35"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
       <c r="O5" s="56"/>
@@ -2617,7 +2625,7 @@
       <c r="X5" s="56"/>
       <c r="Y5" s="56"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="D6" t="s">
         <v>192</v>
       </c>
@@ -2647,7 +2655,7 @@
       <c r="X6" s="35"/>
       <c r="Y6" s="35"/>
     </row>
-    <row r="7" spans="1:26" ht="48">
+    <row r="7" spans="1:26" ht="52" x14ac:dyDescent="0.15">
       <c r="A7" s="46"/>
       <c r="B7" s="51" t="s">
         <v>152</v>
@@ -2699,7 +2707,7 @@
       <c r="Y7" s="35"/>
       <c r="Z7" s="35"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="35" t="s">
         <v>153</v>
       </c>
@@ -2747,7 +2755,7 @@
       <c r="Y8" s="35"/>
       <c r="Z8" s="35"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9" s="35" t="s">
         <v>154</v>
       </c>
@@ -2797,7 +2805,7 @@
       <c r="Y9" s="35"/>
       <c r="Z9" s="35"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
         <v>157</v>
       </c>
@@ -2847,7 +2855,7 @@
       <c r="Y10" s="35"/>
       <c r="Z10" s="35"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11" s="35" t="s">
         <v>172</v>
       </c>
@@ -2895,7 +2903,7 @@
       <c r="Y11" s="35"/>
       <c r="Z11" s="35"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12" s="35" t="s">
         <v>174</v>
       </c>
@@ -2943,7 +2951,7 @@
       <c r="Y12" s="35"/>
       <c r="Z12" s="35"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13" s="52" t="s">
         <v>220</v>
       </c>
@@ -2991,7 +2999,7 @@
       <c r="Y13" s="35"/>
       <c r="Z13" s="35"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14" s="35" t="s">
         <v>173</v>
       </c>
@@ -3039,7 +3047,7 @@
       <c r="Y14" s="35"/>
       <c r="Z14" s="35"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15" s="35" t="s">
         <v>175</v>
       </c>
@@ -3087,7 +3095,7 @@
       <c r="Y15" s="35"/>
       <c r="Z15" s="35"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16" s="52" t="s">
         <v>221</v>
       </c>
@@ -3135,7 +3143,7 @@
       <c r="Y16" s="35"/>
       <c r="Z16" s="35"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17" s="78"/>
       <c r="B17" s="57"/>
       <c r="C17" s="57"/>
@@ -3163,7 +3171,7 @@
       <c r="Y17" s="35"/>
       <c r="Z17" s="35"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A18" s="56"/>
       <c r="M18" s="35"/>
       <c r="N18" s="35"/>
@@ -3179,7 +3187,7 @@
       <c r="X18" s="35"/>
       <c r="Y18" s="35"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="58" t="s">
         <v>160</v>
       </c>
@@ -3197,7 +3205,7 @@
       <c r="X19" s="35"/>
       <c r="Y19" s="35"/>
     </row>
-    <row r="20" spans="1:26" ht="30" customHeight="1">
+    <row r="20" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="88" t="s">
         <v>170</v>
       </c>
@@ -3224,7 +3232,7 @@
       <c r="X20" s="35"/>
       <c r="Y20" s="35"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="K21" s="35"/>
       <c r="L21" s="35"/>
       <c r="M21" s="35"/>
@@ -3239,7 +3247,7 @@
       <c r="V21" s="35"/>
       <c r="W21" s="35"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="K22" s="35"/>
       <c r="L22" s="35"/>
       <c r="M22" s="35"/>
@@ -3254,7 +3262,7 @@
       <c r="V22" s="35"/>
       <c r="W22" s="35"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A23" s="62" t="s">
         <v>171</v>
       </c>
@@ -3281,7 +3289,7 @@
       <c r="V23" s="35"/>
       <c r="W23" s="35"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A24" s="62"/>
       <c r="B24" s="35"/>
       <c r="C24" s="35"/>
@@ -3306,7 +3314,7 @@
       <c r="V24" s="35"/>
       <c r="W24" s="35"/>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A25" s="35" t="s">
         <v>182</v>
       </c>
@@ -3345,7 +3353,7 @@
       <c r="V25" s="35"/>
       <c r="W25" s="35"/>
     </row>
-    <row r="26" spans="1:26" ht="24">
+    <row r="26" spans="1:26" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="46"/>
       <c r="B26" s="46" t="s">
         <v>54</v>
@@ -3387,7 +3395,7 @@
       <c r="U26" s="35"/>
       <c r="V26" s="35"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27" s="35" t="s">
         <v>153</v>
       </c>
@@ -3432,7 +3440,7 @@
       <c r="U27" s="35"/>
       <c r="V27" s="35"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A28" s="35" t="s">
         <v>154</v>
       </c>
@@ -3477,7 +3485,7 @@
       <c r="U28" s="35"/>
       <c r="V28" s="35"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A29" s="35" t="s">
         <v>157</v>
       </c>
@@ -3522,7 +3530,7 @@
       <c r="U29" s="35"/>
       <c r="V29" s="35"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A30" s="35" t="s">
         <v>172</v>
       </c>
@@ -3567,7 +3575,7 @@
       <c r="U30" s="35"/>
       <c r="V30" s="35"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A31" s="35" t="s">
         <v>174</v>
       </c>
@@ -3612,7 +3620,7 @@
       <c r="U31" s="35"/>
       <c r="V31" s="35"/>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A32" s="52" t="s">
         <v>220</v>
       </c>
@@ -3657,7 +3665,7 @@
       <c r="U32" s="35"/>
       <c r="V32" s="35"/>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A33" s="35" t="s">
         <v>173</v>
       </c>
@@ -3703,7 +3711,7 @@
       <c r="U33" s="35"/>
       <c r="V33" s="35"/>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A34" s="35" t="s">
         <v>175</v>
       </c>
@@ -3748,7 +3756,7 @@
       <c r="U34" s="35"/>
       <c r="V34" s="35"/>
     </row>
-    <row r="35" spans="1:23" ht="15" customHeight="1">
+    <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="52" t="s">
         <v>221</v>
       </c>
@@ -3791,7 +3799,7 @@
       <c r="S35" s="35"/>
       <c r="T35" s="35"/>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A36" s="57"/>
       <c r="B36" s="57"/>
       <c r="C36" s="57"/>
@@ -3813,7 +3821,7 @@
       <c r="S36" s="35"/>
       <c r="T36" s="35"/>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
       <c r="K37" s="35"/>
       <c r="L37" s="35"/>
       <c r="M37" s="35"/>
@@ -3828,7 +3836,7 @@
       <c r="V37" s="35"/>
       <c r="W37" s="35"/>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
       <c r="K38" s="35"/>
       <c r="L38" s="35"/>
       <c r="M38" s="35"/>
@@ -3843,7 +3851,7 @@
       <c r="V38" s="35"/>
       <c r="W38" s="35"/>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
       <c r="K39" s="35"/>
       <c r="L39" s="35"/>
       <c r="M39" s="35"/>
@@ -3858,7 +3866,7 @@
       <c r="V39" s="35"/>
       <c r="W39" s="35"/>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>176</v>
       </c>
@@ -3879,11 +3887,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3895,7 +3898,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
@@ -3905,7 +3908,7 @@
     <col min="6" max="6" width="98.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="s">
         <v>39</v>
       </c>
@@ -3915,7 +3918,7 @@
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="38"/>
       <c r="B2" s="32"/>
       <c r="C2" s="33"/>
@@ -3923,7 +3926,7 @@
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="53" t="s">
         <v>162</v>
       </c>
@@ -3933,7 +3936,7 @@
       <c r="E3" s="41"/>
       <c r="F3" s="41"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
@@ -3953,7 +3956,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
         <v>113</v>
       </c>
@@ -3968,7 +3971,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="28" t="s">
         <v>114</v>
       </c>
@@ -3980,7 +3983,7 @@
       <c r="E6" s="43"/>
       <c r="F6" s="42"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>91</v>
       </c>
@@ -3998,7 +4001,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>92</v>
       </c>
@@ -4014,7 +4017,7 @@
       </c>
       <c r="F8" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="53" t="s">
         <v>164</v>
       </c>
@@ -4024,7 +4027,7 @@
       <c r="E10" s="41"/>
       <c r="F10" s="41"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
         <v>0</v>
       </c>
@@ -4044,7 +4047,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12">
+    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="28" t="s">
         <v>113</v>
       </c>
@@ -4059,7 +4062,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="28" t="s">
         <v>114</v>
       </c>
@@ -4071,7 +4074,7 @@
       <c r="E13" s="43"/>
       <c r="F13" s="42"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>91</v>
       </c>
@@ -4089,7 +4092,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>92</v>
       </c>
@@ -4105,7 +4108,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="21"/>
       <c r="C16" s="11"/>
@@ -4113,7 +4116,7 @@
       <c r="E16" s="55"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="53" t="s">
         <v>163</v>
       </c>
@@ -4123,7 +4126,7 @@
       <c r="E17" s="41"/>
       <c r="F17" s="41"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="26" t="s">
         <v>0</v>
       </c>
@@ -4143,7 +4146,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
         <v>113</v>
       </c>
@@ -4159,7 +4162,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="28" t="s">
         <v>114</v>
       </c>
@@ -4171,7 +4174,7 @@
       <c r="E20" s="43"/>
       <c r="F20" s="42"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>91</v>
       </c>
@@ -4189,7 +4192,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>92</v>
       </c>
@@ -4205,7 +4208,7 @@
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="53" t="s">
         <v>116</v>
       </c>
@@ -4215,7 +4218,7 @@
       <c r="E24" s="41"/>
       <c r="F24" s="41"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>0</v>
       </c>
@@ -4235,7 +4238,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="28"/>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -4244,7 +4247,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="28"/>
       <c r="B27" s="44"/>
       <c r="C27" s="28"/>
@@ -4252,7 +4255,7 @@
       <c r="E27" s="43"/>
       <c r="F27" s="42"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="21"/>
       <c r="C28" s="11"/>
@@ -4260,7 +4263,7 @@
       <c r="E28" s="54"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="21"/>
       <c r="C29" s="11"/>
@@ -4271,11 +4274,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4283,22 +4281,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="12" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="17">
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="35"/>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -4311,7 +4309,7 @@
       <c r="J3" s="35"/>
       <c r="K3" s="35"/>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
         <v>169</v>
       </c>
@@ -4326,7 +4324,7 @@
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B5" s="57"/>
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
@@ -4345,7 +4343,7 @@
       <c r="K5" s="57"/>
       <c r="L5" s="57"/>
     </row>
-    <row r="6" spans="1:17" ht="26" customHeight="1">
+    <row r="6" spans="1:17" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="59" t="s">
         <v>131</v>
       </c>
@@ -4379,7 +4377,7 @@
       <c r="K6" s="59"/>
       <c r="L6" s="46"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="47" t="s">
         <v>134</v>
       </c>
@@ -4410,7 +4408,7 @@
       </c>
       <c r="K7" s="47"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" s="47" t="s">
         <v>135</v>
       </c>
@@ -4441,7 +4439,7 @@
       </c>
       <c r="K8" s="47"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" s="47" t="s">
         <v>136</v>
       </c>
@@ -4472,7 +4470,7 @@
       </c>
       <c r="K9" s="47"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" s="47" t="s">
         <v>137</v>
       </c>
@@ -4503,7 +4501,7 @@
       </c>
       <c r="K10" s="47"/>
     </row>
-    <row r="11" spans="1:17" ht="14">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="47" t="s">
         <v>138</v>
       </c>
@@ -4537,7 +4535,7 @@
       <c r="P11" s="85"/>
       <c r="Q11" s="85"/>
     </row>
-    <row r="12" spans="1:17" ht="14">
+    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="47" t="s">
         <v>139</v>
       </c>
@@ -4571,7 +4569,7 @@
       <c r="P12" s="85"/>
       <c r="Q12" s="85"/>
     </row>
-    <row r="13" spans="1:17" ht="14">
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="47" t="s">
         <v>140</v>
       </c>
@@ -4605,7 +4603,7 @@
       <c r="P13" s="85"/>
       <c r="Q13" s="85"/>
     </row>
-    <row r="14" spans="1:17" ht="14">
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="47" t="s">
         <v>141</v>
       </c>
@@ -4645,7 +4643,7 @@
       <c r="P14" s="85"/>
       <c r="Q14" s="85"/>
     </row>
-    <row r="15" spans="1:17" ht="14">
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="47" t="s">
         <v>147</v>
       </c>
@@ -4681,7 +4679,7 @@
       <c r="P15" s="85"/>
       <c r="Q15" s="85"/>
     </row>
-    <row r="16" spans="1:17" ht="14">
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="47" t="s">
         <v>148</v>
       </c>
@@ -4710,7 +4708,7 @@
         <v>83.215649349999993</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="14">
+    <row r="17" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -4739,7 +4737,7 @@
         <v>61.963943200000003</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="14">
+    <row r="18" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -4769,7 +4767,7 @@
         <v>110.57935965</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="14">
+    <row r="19" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -4799,16 +4797,16 @@
         <v>65.133064000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.15">
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.15">
       <c r="K21" s="35"/>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.15">
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:29" ht="26" customHeight="1">
+    <row r="23" spans="1:29" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="45" t="s">
         <v>159</v>
       </c>
@@ -4816,7 +4814,7 @@
       <c r="C23" s="45"/>
       <c r="K23" s="35"/>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.15">
       <c r="B24" s="33" t="s">
         <v>111</v>
       </c>
@@ -4846,7 +4844,7 @@
       </c>
       <c r="K24" s="35"/>
     </row>
-    <row r="25" spans="1:29" ht="36">
+    <row r="25" spans="1:29" ht="39" x14ac:dyDescent="0.15">
       <c r="A25" s="39" t="s">
         <v>0</v>
       </c>
@@ -4896,7 +4894,7 @@
       <c r="AB25" s="81"/>
       <c r="AC25" s="81"/>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A26" s="38" t="s">
         <v>118</v>
       </c>
@@ -4946,7 +4944,7 @@
       <c r="AB26" s="81"/>
       <c r="AC26" s="81"/>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A27" s="38" t="s">
         <v>119</v>
       </c>
@@ -4996,7 +4994,7 @@
       <c r="AB27" s="81"/>
       <c r="AC27" s="81"/>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A28" s="62"/>
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
@@ -5026,7 +5024,7 @@
       <c r="AB28" s="81"/>
       <c r="AC28" s="81"/>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A29" s="35"/>
       <c r="B29" s="52"/>
       <c r="C29" s="52"/>
@@ -5056,7 +5054,7 @@
       <c r="AB29" s="81"/>
       <c r="AC29" s="81"/>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A30" s="34"/>
       <c r="B30" s="37"/>
       <c r="C30" s="32"/>
@@ -5082,7 +5080,7 @@
       <c r="AB30" s="81"/>
       <c r="AC30" s="81"/>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A31" s="34"/>
       <c r="B31" s="37"/>
       <c r="C31" s="32"/>
@@ -5111,7 +5109,7 @@
       <c r="AB31" s="81"/>
       <c r="AC31" s="81"/>
     </row>
-    <row r="32" spans="1:29" ht="12" customHeight="1">
+    <row r="32" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="81"/>
       <c r="C32" s="81"/>
       <c r="D32" s="81"/>
@@ -5137,7 +5135,7 @@
       <c r="AB32" s="81"/>
       <c r="AC32" s="81"/>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>213</v>
       </c>
@@ -5166,7 +5164,7 @@
       <c r="AB33" s="81"/>
       <c r="AC33" s="81"/>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.15">
       <c r="L34" s="81"/>
       <c r="M34" s="81"/>
       <c r="N34" s="81"/>
@@ -5186,7 +5184,7 @@
       <c r="AB34" s="81"/>
       <c r="AC34" s="81"/>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -5209,7 +5207,7 @@
       <c r="AB35" s="81"/>
       <c r="AC35" s="81"/>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.15">
       <c r="L36" s="81"/>
       <c r="M36" s="81"/>
       <c r="N36" s="81"/>
@@ -5229,7 +5227,7 @@
       <c r="AB36" s="81"/>
       <c r="AC36" s="81"/>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.15">
       <c r="L37" s="81"/>
       <c r="M37" s="81"/>
       <c r="N37" s="81"/>
@@ -5255,11 +5253,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5271,25 +5264,20 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5301,14 +5289,9 @@
       <selection activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5320,7 +5303,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
@@ -5330,7 +5313,7 @@
     <col min="6" max="6" width="91.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -5340,7 +5323,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5348,7 +5331,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -5364,7 +5347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
@@ -5376,7 +5359,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" ht="61" customHeight="1">
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -5388,7 +5371,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>45</v>
       </c>
@@ -5398,7 +5381,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="31" customHeight="1">
+    <row r="7" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -5410,7 +5393,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>46</v>
       </c>
@@ -5420,7 +5403,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -5432,7 +5415,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -5442,7 +5425,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>40</v>
       </c>
@@ -5452,7 +5435,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
         <v>45</v>
       </c>
@@ -5462,7 +5445,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
         <v>46</v>
       </c>
@@ -5472,7 +5455,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="3" t="s">
@@ -5482,7 +5465,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -5492,7 +5475,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>52</v>
       </c>
@@ -5502,7 +5485,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>83</v>
       </c>
@@ -5518,7 +5501,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>59</v>
       </c>
@@ -5534,7 +5517,7 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
         <v>66</v>
       </c>
@@ -5546,7 +5529,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
         <v>64</v>
       </c>
@@ -5560,7 +5543,7 @@
       <c r="E20" s="15"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
         <v>65</v>
       </c>
@@ -5572,7 +5555,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
@@ -5584,7 +5567,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>45</v>
       </c>
@@ -5596,7 +5579,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>48</v>
       </c>
@@ -5608,7 +5591,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>49</v>
       </c>
@@ -5618,7 +5601,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="3"/>
@@ -5626,7 +5609,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
@@ -5636,7 +5619,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="8" t="s">
         <v>57</v>
       </c>
@@ -5648,7 +5631,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
@@ -5660,7 +5643,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
         <v>66</v>
       </c>
@@ -5672,7 +5655,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="3"/>
@@ -5680,7 +5663,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
@@ -5690,7 +5673,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
         <v>53</v>
       </c>
@@ -5700,7 +5683,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
         <v>54</v>
       </c>
@@ -5710,7 +5693,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
         <v>55</v>
       </c>
@@ -5720,7 +5703,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>56</v>
       </c>
@@ -5730,7 +5713,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8" t="s">
         <v>54</v>
       </c>
@@ -5740,7 +5723,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
         <v>55</v>
       </c>
@@ -5750,7 +5733,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
         <v>70</v>
       </c>
@@ -5760,7 +5743,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+    <row r="40" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8" t="s">
         <v>54</v>
       </c>
@@ -5770,7 +5753,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="8" t="s">
         <v>71</v>
       </c>
@@ -5782,7 +5765,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
         <v>72</v>
       </c>
@@ -5794,7 +5777,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="3"/>
@@ -5802,7 +5785,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="3"/>
@@ -5810,7 +5793,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="3"/>
@@ -5818,7 +5801,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="3"/>
@@ -5826,7 +5809,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -5837,10 +5820,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added gw transrow function using neural net
</commit_message>
<xml_diff>
--- a/Water Decision Model Data Inputs.xlsx
+++ b/Water Decision Model Data Inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="3060" windowWidth="18340" windowHeight="10340" tabRatio="689" activeTab="3"/>
+    <workbookView xWindow="8820" yWindow="3340" windowWidth="24780" windowHeight="15540" tabRatio="689" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Parameters" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="225">
   <si>
     <t>Parameter</t>
   </si>
@@ -699,6 +699,15 @@
   </si>
   <si>
     <t>Flex_Plant_2_Extension</t>
+  </si>
+  <si>
+    <t>Al Hunayy cm/d</t>
+  </si>
+  <si>
+    <t>K lower bound</t>
+  </si>
+  <si>
+    <t>K upper bound</t>
   </si>
 </sst>
 </file>
@@ -848,7 +857,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="235">
+  <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1084,8 +1093,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1277,8 +1290,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="67" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="235">
+  <cellStyles count="239">
     <cellStyle name="Comma" xfId="67" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1396,6 +1411,8 @@
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1512,6 +1529,8 @@
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="68" builtinId="5"/>
   </cellStyles>
@@ -4279,16 +4298,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC37"/>
+  <dimension ref="A2:AC39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.2">
@@ -5117,7 +5137,9 @@
       <c r="F32" s="90"/>
       <c r="G32" s="90"/>
       <c r="L32" s="81"/>
-      <c r="M32" s="52"/>
+      <c r="M32" s="52" t="s">
+        <v>222</v>
+      </c>
       <c r="N32" s="52"/>
       <c r="O32" s="52"/>
       <c r="P32" s="52"/>
@@ -5146,7 +5168,10 @@
       <c r="F33" s="90"/>
       <c r="G33" s="90"/>
       <c r="L33" s="81"/>
-      <c r="M33" s="52"/>
+      <c r="M33" s="91">
+        <f>124506717/365</f>
+        <v>341114.29315068491</v>
+      </c>
       <c r="N33" s="52"/>
       <c r="O33" s="52"/>
       <c r="P33" s="52"/>
@@ -5166,7 +5191,10 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.15">
       <c r="L34" s="81"/>
-      <c r="M34" s="81"/>
+      <c r="M34" s="61">
+        <f>3989021/365</f>
+        <v>10928.824657534247</v>
+      </c>
       <c r="N34" s="81"/>
       <c r="O34" s="81"/>
       <c r="P34" s="81"/>
@@ -5246,6 +5274,26 @@
       <c r="AA37" s="81"/>
       <c r="AB37" s="81"/>
       <c r="AC37" s="81"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="92">
+        <f>B26/315*365</f>
+        <v>1.9698412698412695E-3</v>
+      </c>
+      <c r="C39" s="92" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5299,7 +5347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>

</xml_diff>